<commit_message>
Update results of 20160404 - 001 -> 004
</commit_message>
<xml_diff>
--- a/20160404 - 001/running_logs/logs.xlsx
+++ b/20160404 - 001/running_logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="43">
   <si>
     <t>Time</t>
   </si>
@@ -101,6 +101,48 @@
   </si>
   <si>
     <t>20160405_093654</t>
+  </si>
+  <si>
+    <t>20160405_130217</t>
+  </si>
+  <si>
+    <t>remove multiple spaces, trim "space" and ",", convert unicode to ascii, convert to lower</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 1000</t>
+  </si>
+  <si>
+    <t>20160405_131125</t>
+  </si>
+  <si>
+    <t>20160405_132056</t>
+  </si>
+  <si>
+    <t>20160405_133039</t>
+  </si>
+  <si>
+    <t>20160405_134027</t>
+  </si>
+  <si>
+    <t>20160405_145007</t>
+  </si>
+  <si>
+    <t>convert unicode to ascii, convert to lower, remove multiple spaces, trim "space" and ","</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 2000</t>
+  </si>
+  <si>
+    <t>20160405_150820</t>
+  </si>
+  <si>
+    <t>20160405_152656</t>
+  </si>
+  <si>
+    <t>20160405_154619</t>
+  </si>
+  <si>
+    <t>20160405_160605</t>
   </si>
 </sst>
 </file>
@@ -432,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -819,6 +861,326 @@
         <v>0.333333333333333</v>
       </c>
     </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>547.1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13">
+        <v>0.993333333333333</v>
+      </c>
+      <c r="H13">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13">
+        <v>0.427083333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>571.652</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14">
+        <v>0.99</v>
+      </c>
+      <c r="H14">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <v>0.427083333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>583.173</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15">
+        <v>0.990666666666667</v>
+      </c>
+      <c r="H15">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>587.907</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16">
+        <v>0.994</v>
+      </c>
+      <c r="H16">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>597.983</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17">
+        <v>0.991333333333333</v>
+      </c>
+      <c r="H17">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>1093.521</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18">
+        <v>0.990666666666667</v>
+      </c>
+      <c r="H18">
+        <v>0.986798679867987</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18">
+        <v>0.326315789473684</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>1116.069</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19">
+        <v>0.99</v>
+      </c>
+      <c r="H19">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>1162.183</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20">
+        <v>0.992666666666667</v>
+      </c>
+      <c r="H20">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <v>1186.798</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21">
+        <v>0.996666666666667</v>
+      </c>
+      <c r="H21">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22">
+        <v>1218.147</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22">
+        <v>0.996</v>
+      </c>
+      <c r="H22">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update results of test case 001 -> 004
</commit_message>
<xml_diff>
--- a/20160404 - 001/running_logs/logs.xlsx
+++ b/20160404 - 001/running_logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="57">
   <si>
     <t>Time</t>
   </si>
@@ -143,6 +143,48 @@
   </si>
   <si>
     <t>20160405_160605</t>
+  </si>
+  <si>
+    <t>20160405_164851</t>
+  </si>
+  <si>
+    <t>convert to lower, convert unicode to ascii, remove multiple spaces, trim "space" and ","</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 4000</t>
+  </si>
+  <si>
+    <t>20160405_172633</t>
+  </si>
+  <si>
+    <t>20160405_180522</t>
+  </si>
+  <si>
+    <t>20160405_184515</t>
+  </si>
+  <si>
+    <t>20160405_192540</t>
+  </si>
+  <si>
+    <t>20160406_081417</t>
+  </si>
+  <si>
+    <t>remove multiple spaces, convert to lower, trim "space" and ",", convert unicode to ascii</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 6000</t>
+  </si>
+  <si>
+    <t>20160406_091105</t>
+  </si>
+  <si>
+    <t>20160406_100808</t>
+  </si>
+  <si>
+    <t>20160406_113349</t>
+  </si>
+  <si>
+    <t>20160406_131042</t>
   </si>
 </sst>
 </file>
@@ -474,7 +516,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1181,6 +1223,326 @@
         <v>0.416666666666667</v>
       </c>
     </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23">
+        <v>2262.705</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23">
+        <v>0.994</v>
+      </c>
+      <c r="H23">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24">
+        <v>2328.383</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24">
+        <v>0.993333333333333</v>
+      </c>
+      <c r="H24">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25">
+        <v>2393.407</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25">
+        <v>0.994666666666667</v>
+      </c>
+      <c r="H25">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25">
+        <v>0.34375</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26">
+        <v>2424.495</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26">
+        <v>0.992666666666667</v>
+      </c>
+      <c r="H26">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27">
+        <v>2421.675</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27">
+        <v>0.99</v>
+      </c>
+      <c r="H27">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>3407.352</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28">
+        <v>0.994</v>
+      </c>
+      <c r="H28">
+        <v>0.986798679867987</v>
+      </c>
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28">
+        <v>0.368421052631579</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29">
+        <v>3422.952</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29">
+        <v>0.991333333333333</v>
+      </c>
+      <c r="H29">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30">
+        <v>5140.958</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30">
+        <v>0.990666666666667</v>
+      </c>
+      <c r="H30">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30">
+        <v>0.385416666666667</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31">
+        <v>5813.335</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31">
+        <v>0.993333333333333</v>
+      </c>
+      <c r="H31">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>7151.665</v>
+      </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32">
+        <v>0.991333333333333</v>
+      </c>
+      <c r="H32">
+        <v>0.99009900990099</v>
+      </c>
+      <c r="I32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32">
+        <v>0.416666666666667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>